<commit_message>
add add html on bin dir
</commit_message>
<xml_diff>
--- a/bin/08...Mood+Study & Analysis/仕様と目標.xlsx
+++ b/bin/08...Mood+Study & Analysis/仕様と目標.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
   <si>
     <t>ここでは、ダーウィンの提唱する進化論に基づき
 『人の由来と性に関連した選択』により提示された証拠を基に
@@ -1124,134 +1124,7 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>あたかも人と会話した事を連想させ、記憶や結果に“会話をした” という解釈が残る機構と判断しています。</t>
-    <rPh sb="10" eb="11">
-      <t>コト</t>
-    </rPh>
-    <rPh sb="17" eb="19">
-      <t>キオク</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ケッカ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>カイワ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>カイシャク</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>キコウ</t>
-    </rPh>
-    <rPh sb="42" eb="44">
-      <t>ハンダン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>人と人工無脳が会話を行う上での目標と、完成形に求めるものは “面白い会話” であり</t>
-    <rPh sb="0" eb="1">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジンコウ</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ム</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ノウ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>カイワ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>オコナ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ウエ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>モクヒョウ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>カンセイ</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>ケイ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>モト</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>オモシロ</t>
-    </rPh>
-    <rPh sb="34" eb="36">
-      <t>カイワ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>話していて飽きない “使用者が楽しめる会話”であり、気を使わず“寂しさを感じさせない”ものです。</t>
-    <rPh sb="0" eb="1">
-      <t>ハナ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="26" eb="27">
-      <t>キ</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>サミ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>カン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>前向きな結果への貢献を製作の目標としています。</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>解決や推論といった知的活動は、暗に人は嫌悪している節がある事に由来している為です。</t>
-    <rPh sb="0" eb="2">
-      <t>カイケツ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>スイロン</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>チテキ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
-      <t>カツドウ</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>アン</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>ヒト</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ケンオ</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>フシ</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>コト</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>ユライ</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>タメ</t>
-    </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -1306,37 +1179,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>そこに、知的活動は必要としておらず、使用者の感情出力に楽しさや満足感・充実感といった</t>
-    <rPh sb="4" eb="6">
-      <t>チテキ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>カツドウ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="18" eb="21">
-      <t>シヨウシャ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>カンジョウ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>シュツリョク</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>タノ</t>
-    </rPh>
-    <rPh sb="31" eb="34">
-      <t>マンゾクカン</t>
-    </rPh>
-    <rPh sb="35" eb="38">
-      <t>ジュウジツカン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>実装する上での目標は以下の要件を満たすものとします。</t>
     <rPh sb="0" eb="2">
       <t>ジッソウ</t>
@@ -1891,6 +1733,113 @@
   </si>
   <si>
     <t>単語感情極性対応表</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t>あたかも人と</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>会話した事を連想</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>させ、</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>記憶や結果に“会話をした” という解釈が残る機構</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>と判断しています。</t>
+    </r>
+    <rPh sb="10" eb="11">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>キオク</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ケッカ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>カイワ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>カイシャク</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>キコウ</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ハンダン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>主となる目標に、知的活動は必要としておらず、使用者の感情出力に楽しさや満足感・充実感といった</t>
+    <rPh sb="0" eb="1">
+      <t>シュ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>モクヒョウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>チテキ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>カツドウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="22" eb="25">
+      <t>シヨウシャ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>カンジョウ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>シュツリョク</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>タノ</t>
+    </rPh>
+    <rPh sb="35" eb="38">
+      <t>マンゾクカン</t>
+    </rPh>
+    <rPh sb="39" eb="42">
+      <t>ジュウジツカン</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1898,7 +1847,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1970,6 +1919,32 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -2452,7 +2427,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2510,7 +2486,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2529,59 +2504,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>258537</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>349252</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>48025</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="図 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7062108" y="0"/>
-          <a:ext cx="4172858" cy="3129643"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>578303</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>616403</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>567941</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>70757</xdr:rowOff>
+      <xdr:colOff>606041</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>51707</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2598,7 +2530,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5378903" y="7086600"/>
+          <a:off x="5417003" y="1066800"/>
           <a:ext cx="4104438" cy="3956957"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2652,11 +2584,15 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3600"/>
+            <a:t>Program</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3600"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2943,7 +2879,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3292,8 +3228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3351,7 +3287,7 @@
     </row>
     <row r="12" spans="2:3" ht="15" customHeight="1">
       <c r="C12" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" customHeight="1">
@@ -3415,7 +3351,7 @@
     </row>
     <row r="28" spans="2:3" ht="15" customHeight="1">
       <c r="C28" s="1" t="s">
-        <v>65</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15" customHeight="1"/>
@@ -3425,31 +3361,19 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="15" customHeight="1">
-      <c r="C32" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" ht="15" customHeight="1">
-      <c r="C33" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
+    <row r="32" spans="2:3" ht="15" customHeight="1"/>
+    <row r="33" spans="3:3" ht="15" customHeight="1"/>
     <row r="34" spans="3:3" ht="15" customHeight="1">
       <c r="C34" s="1" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="3:3" ht="15" customHeight="1">
       <c r="C35" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" ht="15" customHeight="1">
-      <c r="C36" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" ht="15" customHeight="1"/>
     <row r="37" spans="3:3" ht="15" customHeight="1"/>
     <row r="38" spans="3:3" ht="15" customHeight="1"/>
     <row r="39" spans="3:3" ht="15" customHeight="1"/>
@@ -3458,7 +3382,6 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3466,8 +3389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B6:F32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3477,97 +3400,97 @@
   <sheetData>
     <row r="6" spans="2:6">
       <c r="F6" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="F10" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3606,10 +3529,10 @@
       <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="34"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="4"/>
       <c r="I2" s="3" t="s">
         <v>21</v>
@@ -3620,10 +3543,10 @@
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="4"/>
       <c r="I3" s="3" t="s">
         <v>22</v>
@@ -3631,11 +3554,11 @@
     </row>
     <row r="4" spans="1:9" ht="96" customHeight="1" thickBot="1">
       <c r="A4" s="24"/>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="4"/>
       <c r="I4" s="3" t="s">
         <v>23</v>
@@ -3652,14 +3575,14 @@
     </row>
     <row r="6" spans="1:9" ht="19.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="19.5" customHeight="1">
@@ -3676,10 +3599,10 @@
       <c r="E7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="48"/>
+      <c r="G7" s="49"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:9" ht="19.5" customHeight="1">
@@ -3696,10 +3619,10 @@
       <c r="E8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="44"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="19.5" customHeight="1">
@@ -3716,10 +3639,10 @@
       <c r="E9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="44"/>
+      <c r="G9" s="45"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:9" ht="19.5" customHeight="1">
@@ -3736,10 +3659,10 @@
       <c r="E10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="44"/>
+      <c r="G10" s="45"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:9" ht="19.5" customHeight="1">
@@ -3756,10 +3679,10 @@
       <c r="E11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="44"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:9" ht="19.5" customHeight="1">
@@ -3776,10 +3699,10 @@
       <c r="E12" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="44"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" customHeight="1">
@@ -3796,10 +3719,10 @@
       <c r="E13" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="44"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:9" ht="19.5" customHeight="1" thickBot="1">
@@ -3816,10 +3739,10 @@
       <c r="E14" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="46"/>
+      <c r="G14" s="47"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="19.5" customHeight="1" thickTop="1">
@@ -3849,124 +3772,124 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="2:9" ht="75" customHeight="1">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
     </row>
     <row r="19" spans="2:9" ht="19.5" customHeight="1"/>
     <row r="20" spans="2:9">
-      <c r="B20" s="49" t="s">
-        <v>121</v>
+      <c r="B20" s="29" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="49" t="s">
-        <v>123</v>
+      <c r="B22" s="29" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="49" t="s">
-        <v>124</v>
+      <c r="B24" s="29" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="2:9">
-      <c r="B26" s="49" t="s">
-        <v>126</v>
+      <c r="B26" s="29" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="2:9">
       <c r="B27" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="B28" s="49" t="s">
-        <v>129</v>
+      <c r="B28" s="29" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="2:9">
-      <c r="B30" s="49" t="s">
-        <v>131</v>
+      <c r="B30" s="29" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:9">
-      <c r="B32" s="49" t="s">
-        <v>132</v>
+      <c r="B32" s="29" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="49" t="s">
-        <v>134</v>
+      <c r="B34" s="29" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="2:2">
-      <c r="B36" s="49" t="s">
-        <v>136</v>
+      <c r="B36" s="29" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="2:2">
-      <c r="B38" s="49" t="s">
-        <v>138</v>
+      <c r="B38" s="29" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="2:2">
-      <c r="B40" s="49" t="s">
-        <v>141</v>
+      <c r="B40" s="29" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="2:2">
       <c r="B41" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3994,10 +3917,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B52"/>
+  <dimension ref="B3:B43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4005,149 +3928,149 @@
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" ht="18.75">
-      <c r="B3" s="29" t="s">
-        <v>91</v>
+    <row r="3" spans="2:2" ht="24">
+      <c r="B3" s="30" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="1" t="s">
-        <v>97</v>
+      <c r="B4" s="29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="2:2">
-      <c r="B6" s="1" t="s">
-        <v>95</v>
+      <c r="B6" s="29" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="2:2">
-      <c r="B8" s="1" t="s">
-        <v>98</v>
+      <c r="B8" s="29" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:2">
-      <c r="B10" s="1" t="s">
-        <v>100</v>
+      <c r="B10" s="29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:2">
-      <c r="B12" s="1" t="s">
-        <v>102</v>
+      <c r="B12" s="29" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="1" t="s">
-        <v>105</v>
+      <c r="B14" s="29" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:2">
-      <c r="B16" s="1" t="s">
-        <v>107</v>
+      <c r="B16" s="29" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="24">
+      <c r="B22" s="30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="18.75">
-      <c r="B31" s="29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="1" t="s">
-        <v>94</v>
+    <row r="29" spans="2:2">
+      <c r="B29" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="1" t="s">
-        <v>110</v>
+      <c r="B34" s="29" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" ht="24">
+      <c r="B41" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="1" t="s">
-        <v>116</v>
+    <row r="42" spans="2:2">
+      <c r="B42" s="29" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="2:2">
       <c r="B43" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" ht="18.75">
-      <c r="B50" s="29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>